<commit_message>
removed woman's hgt & wgt
Women's MUAC for PLW is preferred
</commit_message>
<xml_diff>
--- a/ACO_SMART_Survey_2022.xlsx
+++ b/ACO_SMART_Survey_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unicef-my.sharepoint.com/personal/rojohnston_unicef_org1/Documents/1 UNICEF Work/1 Afghanistan/Surveys/UrbanSMART/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB600E9D-3F34-4F47-9E4F-449300B8EA05}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{BB600E9D-3F34-4F47-9E4F-449300B8EA05}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{ABF401B7-2C71-4CE1-BA52-F6743077993A}"/>
   <bookViews>
-    <workbookView xWindow="12180" yWindow="-11640" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="11592" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1261" uniqueCount="802">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="790">
   <si>
     <t>type</t>
   </si>
@@ -1580,9 +1580,6 @@
     <t>measles</t>
   </si>
   <si>
-    <t>Has the child  ${child_name}  received a measles vaccination?</t>
-  </si>
-  <si>
     <t>آیا کودک ${child_name} واکسن سرخکان دریافت کرده است؟</t>
   </si>
   <si>
@@ -1841,42 +1838,6 @@
     <t>Please remeasure woman's MUAC</t>
   </si>
   <si>
-    <t>wom_hgt</t>
-  </si>
-  <si>
-    <t>Woman's HEIGHT in CM of ${wom_name}</t>
-  </si>
-  <si>
-    <t>قد زن در سانتی متر ${wom_name}</t>
-  </si>
-  <si>
-    <t>د ښځې لوړوالی د ${wom_name} په سانتی متر کې</t>
-  </si>
-  <si>
-    <t>(. &gt;= 110 and . &lt;210)</t>
-  </si>
-  <si>
-    <t>Please remeasure woman's HEIGHT</t>
-  </si>
-  <si>
-    <t>wom_wgt</t>
-  </si>
-  <si>
-    <t>Woman's WEIGHT in KG of ${wom_name}</t>
-  </si>
-  <si>
-    <t>وزن زن به کیلوگرم ${wom_name}</t>
-  </si>
-  <si>
-    <t>د ښځې وزن ${wom_name}  کیلوګرام کې</t>
-  </si>
-  <si>
-    <t>(. &gt;= 25 and . &lt;200)</t>
-  </si>
-  <si>
-    <t>Please remeasure woman's WEIGHT</t>
-  </si>
-  <si>
     <t>location</t>
   </si>
   <si>
@@ -1892,9 +1853,6 @@
     <t>مهرباني وکړئ د GPS لوستل واخلئ</t>
   </si>
   <si>
-    <t>Push the 'Save GeoPoint' button when the accuracy of the GPS measure is less than 25 m. Avoid taking it inside house or under trees (to make it faster).</t>
-  </si>
-  <si>
     <t>هتگامی که دقت اندازه گیری GPS کمتر از 25 متر باشد، دکمه "Save GeoPoint" را فشار دهید. از ګرفتن آن در داخل خانه یا زیر درختان خودداری کنید (برای سرعت بخشیدن به آن).</t>
   </si>
   <si>
@@ -2610,6 +2568,12 @@
   </si>
   <si>
     <t>English</t>
+  </si>
+  <si>
+    <t>Has the child  ${child_name} received a measles vaccination?</t>
+  </si>
+  <si>
+    <t>Push the 'Save GeoPoint' button when standing outside of selected household. Avoid taking it inside house or under trees (to make it faster).</t>
   </si>
 </sst>
 </file>
@@ -2996,7 +2960,7 @@
   <dimension ref="A1:R186"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="A164" sqref="A164:XFD164"/>
+      <selection activeCell="F171" sqref="F171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5411,22 +5375,22 @@
         <v>457</v>
       </c>
       <c r="C143" t="s">
+        <v>788</v>
+      </c>
+      <c r="D143" t="s">
         <v>458</v>
       </c>
-      <c r="D143" t="s">
+      <c r="E143" t="s">
         <v>459</v>
       </c>
-      <c r="E143" t="s">
+      <c r="F143" t="s">
         <v>460</v>
       </c>
-      <c r="F143" t="s">
+      <c r="G143" t="s">
         <v>461</v>
       </c>
-      <c r="G143" t="s">
+      <c r="H143" t="s">
         <v>462</v>
-      </c>
-      <c r="H143" t="s">
-        <v>463</v>
       </c>
       <c r="M143" t="s">
         <v>456</v>
@@ -5437,19 +5401,19 @@
         <v>106</v>
       </c>
       <c r="B144" t="s">
+        <v>463</v>
+      </c>
+      <c r="C144" t="s">
         <v>464</v>
       </c>
-      <c r="C144" t="s">
+      <c r="D144" t="s">
         <v>465</v>
       </c>
-      <c r="D144" t="s">
+      <c r="E144" t="s">
         <v>466</v>
       </c>
-      <c r="E144" t="s">
+      <c r="M144" t="s">
         <v>467</v>
-      </c>
-      <c r="M144" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="145" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -5457,19 +5421,19 @@
         <v>106</v>
       </c>
       <c r="B145" t="s">
+        <v>468</v>
+      </c>
+      <c r="C145" t="s">
         <v>469</v>
       </c>
-      <c r="C145" t="s">
+      <c r="D145" t="s">
         <v>470</v>
       </c>
-      <c r="D145" t="s">
+      <c r="E145" t="s">
         <v>471</v>
       </c>
-      <c r="E145" t="s">
-        <v>472</v>
-      </c>
       <c r="M145" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="146" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -5477,19 +5441,19 @@
         <v>106</v>
       </c>
       <c r="B146" t="s">
+        <v>472</v>
+      </c>
+      <c r="C146" t="s">
         <v>473</v>
       </c>
-      <c r="C146" t="s">
+      <c r="D146" t="s">
         <v>474</v>
       </c>
-      <c r="D146" t="s">
+      <c r="E146" t="s">
         <v>475</v>
       </c>
-      <c r="E146" t="s">
-        <v>476</v>
-      </c>
       <c r="M146" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="147" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -5497,13 +5461,13 @@
         <v>21</v>
       </c>
       <c r="B147" t="s">
+        <v>476</v>
+      </c>
+      <c r="I147" t="s">
         <v>477</v>
       </c>
-      <c r="I147" t="s">
+      <c r="M147" t="s">
         <v>478</v>
-      </c>
-      <c r="M147" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="148" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -5511,13 +5475,13 @@
         <v>21</v>
       </c>
       <c r="B148" t="s">
+        <v>479</v>
+      </c>
+      <c r="I148" t="s">
+        <v>477</v>
+      </c>
+      <c r="M148" t="s">
         <v>480</v>
-      </c>
-      <c r="I148" t="s">
-        <v>478</v>
-      </c>
-      <c r="M148" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="149" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -5525,28 +5489,28 @@
         <v>59</v>
       </c>
       <c r="B149" t="s">
+        <v>481</v>
+      </c>
+      <c r="C149" t="s">
         <v>482</v>
       </c>
-      <c r="C149" t="s">
+      <c r="D149" t="s">
         <v>483</v>
       </c>
-      <c r="D149" t="s">
+      <c r="E149" t="s">
         <v>484</v>
       </c>
-      <c r="E149" t="s">
+      <c r="F149" t="s">
         <v>485</v>
       </c>
-      <c r="F149" t="s">
+      <c r="G149" t="s">
         <v>486</v>
       </c>
-      <c r="G149" t="s">
+      <c r="H149" t="s">
         <v>487</v>
       </c>
-      <c r="H149" t="s">
+      <c r="M149" t="s">
         <v>488</v>
-      </c>
-      <c r="M149" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="150" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -5554,19 +5518,19 @@
         <v>106</v>
       </c>
       <c r="B150" t="s">
+        <v>489</v>
+      </c>
+      <c r="C150" t="s">
         <v>490</v>
       </c>
-      <c r="C150" t="s">
+      <c r="D150" t="s">
         <v>491</v>
       </c>
-      <c r="D150" t="s">
+      <c r="E150" t="s">
         <v>492</v>
       </c>
-      <c r="E150" t="s">
-        <v>493</v>
-      </c>
       <c r="M150" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="151" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -5574,28 +5538,28 @@
         <v>59</v>
       </c>
       <c r="B151" t="s">
+        <v>493</v>
+      </c>
+      <c r="C151" t="s">
         <v>494</v>
       </c>
-      <c r="C151" t="s">
+      <c r="D151" t="s">
         <v>495</v>
       </c>
-      <c r="D151" t="s">
+      <c r="E151" t="s">
         <v>496</v>
       </c>
-      <c r="E151" t="s">
+      <c r="F151" t="s">
         <v>497</v>
       </c>
-      <c r="F151" t="s">
+      <c r="G151" t="s">
         <v>498</v>
       </c>
-      <c r="G151" t="s">
+      <c r="H151" t="s">
         <v>499</v>
       </c>
-      <c r="H151" t="s">
+      <c r="M151" t="s">
         <v>500</v>
-      </c>
-      <c r="M151" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="152" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -5603,19 +5567,19 @@
         <v>106</v>
       </c>
       <c r="B152" t="s">
+        <v>501</v>
+      </c>
+      <c r="C152" t="s">
         <v>502</v>
       </c>
-      <c r="C152" t="s">
+      <c r="D152" t="s">
         <v>503</v>
       </c>
-      <c r="D152" t="s">
+      <c r="E152" t="s">
         <v>504</v>
       </c>
-      <c r="E152" t="s">
-        <v>505</v>
-      </c>
       <c r="M152" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="153" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -5623,13 +5587,13 @@
         <v>21</v>
       </c>
       <c r="B153" t="s">
+        <v>505</v>
+      </c>
+      <c r="I153" t="s">
+        <v>477</v>
+      </c>
+      <c r="M153" t="s">
         <v>506</v>
-      </c>
-      <c r="I153" t="s">
-        <v>478</v>
-      </c>
-      <c r="M153" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="154" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -5637,13 +5601,13 @@
         <v>21</v>
       </c>
       <c r="B154" t="s">
+        <v>507</v>
+      </c>
+      <c r="I154" t="s">
+        <v>477</v>
+      </c>
+      <c r="M154" t="s">
         <v>508</v>
-      </c>
-      <c r="I154" t="s">
-        <v>478</v>
-      </c>
-      <c r="M154" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="155" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -5651,13 +5615,13 @@
         <v>21</v>
       </c>
       <c r="B155" t="s">
+        <v>509</v>
+      </c>
+      <c r="I155" t="s">
+        <v>477</v>
+      </c>
+      <c r="M155" t="s">
         <v>510</v>
-      </c>
-      <c r="I155" t="s">
-        <v>478</v>
-      </c>
-      <c r="M155" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="156" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -5665,13 +5629,13 @@
         <v>21</v>
       </c>
       <c r="B156" t="s">
+        <v>511</v>
+      </c>
+      <c r="I156" t="s">
+        <v>477</v>
+      </c>
+      <c r="M156" t="s">
         <v>512</v>
-      </c>
-      <c r="I156" t="s">
-        <v>478</v>
-      </c>
-      <c r="M156" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="157" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -5687,13 +5651,13 @@
         <v>73</v>
       </c>
       <c r="B158" t="s">
+        <v>513</v>
+      </c>
+      <c r="C158" t="s">
         <v>514</v>
       </c>
-      <c r="C158" t="s">
+      <c r="R158" t="s">
         <v>515</v>
-      </c>
-      <c r="R158" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="159" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -5701,7 +5665,7 @@
         <v>21</v>
       </c>
       <c r="B159" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I159" t="s">
         <v>133</v>
@@ -5712,10 +5676,10 @@
         <v>21</v>
       </c>
       <c r="B160" t="s">
+        <v>517</v>
+      </c>
+      <c r="I160" t="s">
         <v>518</v>
-      </c>
-      <c r="I160" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="161" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5723,10 +5687,10 @@
         <v>21</v>
       </c>
       <c r="B161" t="s">
+        <v>519</v>
+      </c>
+      <c r="I161" t="s">
         <v>520</v>
-      </c>
-      <c r="I161" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="162" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5734,10 +5698,10 @@
         <v>21</v>
       </c>
       <c r="B162" t="s">
+        <v>521</v>
+      </c>
+      <c r="I162" t="s">
         <v>522</v>
-      </c>
-      <c r="I162" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="163" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5745,19 +5709,19 @@
         <v>59</v>
       </c>
       <c r="B163" t="s">
+        <v>523</v>
+      </c>
+      <c r="C163" t="s">
         <v>524</v>
       </c>
-      <c r="C163" t="s">
+      <c r="D163" t="s">
         <v>525</v>
       </c>
-      <c r="D163" t="s">
+      <c r="E163" t="s">
         <v>526</v>
       </c>
-      <c r="E163" t="s">
+      <c r="M163" t="s">
         <v>527</v>
-      </c>
-      <c r="M163" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="165" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5765,19 +5729,19 @@
         <v>106</v>
       </c>
       <c r="B165" t="s">
+        <v>528</v>
+      </c>
+      <c r="C165" t="s">
         <v>529</v>
       </c>
-      <c r="C165" t="s">
+      <c r="D165" t="s">
         <v>530</v>
       </c>
-      <c r="D165" t="s">
+      <c r="E165" t="s">
         <v>531</v>
       </c>
-      <c r="E165" t="s">
-        <v>532</v>
-      </c>
       <c r="M165" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="166" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5785,115 +5749,51 @@
         <v>106</v>
       </c>
       <c r="B166" t="s">
+        <v>532</v>
+      </c>
+      <c r="C166" t="s">
         <v>533</v>
       </c>
-      <c r="C166" t="s">
+      <c r="D166" t="s">
         <v>534</v>
       </c>
-      <c r="D166" t="s">
+      <c r="E166" t="s">
         <v>535</v>
       </c>
-      <c r="E166" t="s">
-        <v>536</v>
-      </c>
       <c r="M166" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="167" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" t="s">
+        <v>536</v>
+      </c>
+      <c r="B167" t="s">
         <v>537</v>
       </c>
-      <c r="B167" t="s">
+      <c r="C167" t="s">
         <v>538</v>
       </c>
-      <c r="C167" t="s">
+      <c r="D167" t="s">
         <v>539</v>
       </c>
-      <c r="D167" t="s">
+      <c r="E167" t="s">
         <v>540</v>
       </c>
-      <c r="E167" t="s">
+      <c r="L167" t="s">
         <v>541</v>
       </c>
-      <c r="L167" t="s">
+      <c r="M167" t="s">
         <v>542</v>
       </c>
-      <c r="M167" t="s">
+      <c r="N167" t="s">
         <v>543</v>
       </c>
-      <c r="N167" t="s">
-        <v>544</v>
-      </c>
       <c r="O167" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="P167" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="168" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A168" t="s">
-        <v>537</v>
-      </c>
-      <c r="B168" t="s">
-        <v>545</v>
-      </c>
-      <c r="C168" t="s">
-        <v>546</v>
-      </c>
-      <c r="D168" t="s">
-        <v>547</v>
-      </c>
-      <c r="E168" t="s">
-        <v>548</v>
-      </c>
-      <c r="L168" t="s">
-        <v>549</v>
-      </c>
-      <c r="M168" t="s">
         <v>543</v>
-      </c>
-      <c r="N168" t="s">
-        <v>550</v>
-      </c>
-      <c r="O168" t="s">
-        <v>550</v>
-      </c>
-      <c r="P168" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="169" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A169" t="s">
-        <v>537</v>
-      </c>
-      <c r="B169" t="s">
-        <v>551</v>
-      </c>
-      <c r="C169" t="s">
-        <v>552</v>
-      </c>
-      <c r="D169" t="s">
-        <v>553</v>
-      </c>
-      <c r="E169" t="s">
-        <v>554</v>
-      </c>
-      <c r="L169" t="s">
-        <v>555</v>
-      </c>
-      <c r="M169" t="s">
-        <v>543</v>
-      </c>
-      <c r="N169" t="s">
-        <v>556</v>
-      </c>
-      <c r="O169" t="s">
-        <v>556</v>
-      </c>
-      <c r="P169" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="170" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5901,123 +5801,123 @@
         <v>103</v>
       </c>
       <c r="B170" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="171" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" t="s">
-        <v>557</v>
+        <v>544</v>
       </c>
       <c r="B171" t="s">
-        <v>558</v>
+        <v>545</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>559</v>
+        <v>546</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>560</v>
+        <v>547</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>561</v>
+        <v>548</v>
       </c>
       <c r="F171" s="1" t="s">
-        <v>562</v>
+        <v>789</v>
       </c>
       <c r="G171" s="1" t="s">
-        <v>563</v>
+        <v>549</v>
       </c>
       <c r="H171" s="1" t="s">
-        <v>564</v>
+        <v>550</v>
       </c>
     </row>
     <row r="172" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" t="s">
-        <v>565</v>
+        <v>551</v>
       </c>
       <c r="B172" t="s">
-        <v>566</v>
+        <v>552</v>
       </c>
       <c r="C172" t="s">
-        <v>567</v>
+        <v>553</v>
       </c>
       <c r="D172" t="s">
-        <v>568</v>
+        <v>554</v>
       </c>
       <c r="E172" t="s">
-        <v>569</v>
+        <v>555</v>
       </c>
       <c r="F172" t="s">
-        <v>570</v>
+        <v>556</v>
       </c>
       <c r="G172" t="s">
-        <v>571</v>
+        <v>557</v>
       </c>
       <c r="H172" t="s">
-        <v>572</v>
+        <v>558</v>
       </c>
       <c r="J172" t="s">
         <v>29</v>
       </c>
       <c r="M172" t="s">
-        <v>573</v>
+        <v>559</v>
       </c>
     </row>
     <row r="173" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" t="s">
-        <v>574</v>
+        <v>560</v>
       </c>
       <c r="B173" t="s">
-        <v>575</v>
+        <v>561</v>
       </c>
       <c r="C173" t="s">
-        <v>567</v>
+        <v>553</v>
       </c>
       <c r="D173" t="s">
-        <v>568</v>
+        <v>554</v>
       </c>
       <c r="E173" t="s">
-        <v>569</v>
+        <v>555</v>
       </c>
       <c r="F173" t="s">
-        <v>570</v>
+        <v>556</v>
       </c>
       <c r="G173" t="s">
-        <v>571</v>
+        <v>557</v>
       </c>
       <c r="H173" t="s">
-        <v>572</v>
+        <v>558</v>
       </c>
       <c r="M173" t="s">
-        <v>576</v>
+        <v>562</v>
       </c>
     </row>
     <row r="174" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" t="s">
-        <v>577</v>
+        <v>563</v>
       </c>
       <c r="B174" t="s">
-        <v>578</v>
+        <v>564</v>
       </c>
       <c r="C174" t="s">
-        <v>567</v>
+        <v>553</v>
       </c>
       <c r="D174" t="s">
-        <v>568</v>
+        <v>554</v>
       </c>
       <c r="E174" t="s">
-        <v>569</v>
+        <v>555</v>
       </c>
       <c r="G174" t="s">
-        <v>571</v>
+        <v>557</v>
       </c>
       <c r="H174" t="s">
-        <v>572</v>
+        <v>558</v>
       </c>
       <c r="J174" t="s">
         <v>29</v>
       </c>
       <c r="M174" t="s">
-        <v>579</v>
+        <v>565</v>
       </c>
     </row>
     <row r="175" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -6025,19 +5925,19 @@
         <v>59</v>
       </c>
       <c r="B175" t="s">
-        <v>580</v>
+        <v>566</v>
       </c>
       <c r="C175" t="s">
-        <v>581</v>
+        <v>567</v>
       </c>
       <c r="D175" t="s">
-        <v>582</v>
+        <v>568</v>
       </c>
       <c r="E175" t="s">
-        <v>583</v>
+        <v>569</v>
       </c>
       <c r="M175" t="s">
-        <v>584</v>
+        <v>570</v>
       </c>
     </row>
     <row r="176" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -6045,16 +5945,16 @@
         <v>30</v>
       </c>
       <c r="B176" t="s">
-        <v>585</v>
+        <v>571</v>
       </c>
       <c r="C176" t="s">
-        <v>586</v>
+        <v>572</v>
       </c>
       <c r="D176" t="s">
-        <v>587</v>
+        <v>573</v>
       </c>
       <c r="E176" t="s">
-        <v>588</v>
+        <v>574</v>
       </c>
     </row>
     <row r="177" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -6070,10 +5970,10 @@
         <v>21</v>
       </c>
       <c r="B178" t="s">
-        <v>589</v>
+        <v>575</v>
       </c>
       <c r="I178" t="s">
-        <v>590</v>
+        <v>576</v>
       </c>
     </row>
     <row r="180" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -6081,10 +5981,10 @@
         <v>21</v>
       </c>
       <c r="B180" t="s">
-        <v>591</v>
+        <v>577</v>
       </c>
       <c r="I180" t="s">
-        <v>592</v>
+        <v>578</v>
       </c>
     </row>
     <row r="181" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -6092,10 +5992,10 @@
         <v>21</v>
       </c>
       <c r="B181" t="s">
-        <v>593</v>
+        <v>579</v>
       </c>
       <c r="I181" t="s">
-        <v>594</v>
+        <v>580</v>
       </c>
     </row>
     <row r="182" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -6103,10 +6003,10 @@
         <v>21</v>
       </c>
       <c r="B182" t="s">
-        <v>595</v>
+        <v>581</v>
       </c>
       <c r="I182" t="s">
-        <v>596</v>
+        <v>582</v>
       </c>
     </row>
     <row r="183" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -6114,10 +6014,10 @@
         <v>21</v>
       </c>
       <c r="B183" t="s">
-        <v>597</v>
+        <v>583</v>
       </c>
       <c r="I183" t="s">
-        <v>598</v>
+        <v>584</v>
       </c>
     </row>
     <row r="184" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -6125,10 +6025,10 @@
         <v>21</v>
       </c>
       <c r="B184" t="s">
-        <v>599</v>
+        <v>585</v>
       </c>
       <c r="I184" t="s">
-        <v>600</v>
+        <v>586</v>
       </c>
     </row>
     <row r="185" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -6136,10 +6036,10 @@
         <v>21</v>
       </c>
       <c r="B185" t="s">
-        <v>601</v>
+        <v>587</v>
       </c>
       <c r="I185" t="s">
-        <v>602</v>
+        <v>588</v>
       </c>
     </row>
     <row r="186" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -6147,13 +6047,13 @@
         <v>21</v>
       </c>
       <c r="B186" t="s">
-        <v>603</v>
+        <v>589</v>
       </c>
       <c r="I186" t="s">
-        <v>604</v>
+        <v>590</v>
       </c>
       <c r="Q186" t="s">
-        <v>601</v>
+        <v>587</v>
       </c>
     </row>
   </sheetData>
@@ -6171,7 +6071,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>605</v>
+        <v>591</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -6188,53 +6088,53 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>606</v>
+        <v>592</v>
       </c>
       <c r="B2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C2" t="s">
-        <v>607</v>
+        <v>593</v>
       </c>
       <c r="D2" t="s">
-        <v>608</v>
+        <v>594</v>
       </c>
       <c r="E2" t="s">
-        <v>609</v>
+        <v>595</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>606</v>
+        <v>592</v>
       </c>
       <c r="B3" t="s">
-        <v>610</v>
+        <v>596</v>
       </c>
       <c r="C3" t="s">
-        <v>611</v>
+        <v>597</v>
       </c>
       <c r="D3" t="s">
-        <v>612</v>
+        <v>598</v>
       </c>
       <c r="E3" t="s">
-        <v>613</v>
+        <v>599</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>614</v>
+        <v>600</v>
       </c>
       <c r="B4" t="s">
-        <v>614</v>
+        <v>600</v>
       </c>
       <c r="C4" t="s">
-        <v>614</v>
+        <v>600</v>
       </c>
       <c r="D4" t="s">
-        <v>615</v>
+        <v>601</v>
       </c>
       <c r="E4" t="s">
-        <v>615</v>
+        <v>601</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -6242,16 +6142,16 @@
         <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C5" t="s">
-        <v>616</v>
+        <v>602</v>
       </c>
       <c r="D5" t="s">
-        <v>617</v>
+        <v>603</v>
       </c>
       <c r="E5" t="s">
-        <v>618</v>
+        <v>604</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -6259,16 +6159,16 @@
         <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>610</v>
+        <v>596</v>
       </c>
       <c r="C6" t="s">
-        <v>619</v>
+        <v>605</v>
       </c>
       <c r="D6" t="s">
-        <v>620</v>
+        <v>606</v>
       </c>
       <c r="E6" t="s">
-        <v>621</v>
+        <v>607</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -6276,985 +6176,985 @@
         <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>622</v>
+        <v>608</v>
       </c>
       <c r="C7" t="s">
-        <v>623</v>
+        <v>609</v>
       </c>
       <c r="D7" t="s">
-        <v>624</v>
+        <v>610</v>
       </c>
       <c r="E7" t="s">
-        <v>625</v>
+        <v>611</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B8" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C8" t="s">
-        <v>627</v>
+        <v>613</v>
       </c>
       <c r="D8" t="s">
-        <v>628</v>
+        <v>614</v>
       </c>
       <c r="E8" t="s">
-        <v>628</v>
+        <v>614</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B9" t="s">
-        <v>610</v>
+        <v>596</v>
       </c>
       <c r="C9" t="s">
-        <v>629</v>
+        <v>615</v>
       </c>
       <c r="D9" t="s">
-        <v>630</v>
+        <v>616</v>
       </c>
       <c r="E9" t="s">
-        <v>630</v>
+        <v>616</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B10" t="s">
-        <v>622</v>
+        <v>608</v>
       </c>
       <c r="C10" t="s">
-        <v>631</v>
+        <v>617</v>
       </c>
       <c r="D10" t="s">
-        <v>632</v>
+        <v>618</v>
       </c>
       <c r="E10" t="s">
-        <v>632</v>
+        <v>618</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B11" t="s">
-        <v>633</v>
+        <v>619</v>
       </c>
       <c r="C11" t="s">
-        <v>634</v>
+        <v>620</v>
       </c>
       <c r="D11" t="s">
-        <v>635</v>
+        <v>621</v>
       </c>
       <c r="E11" t="s">
-        <v>635</v>
+        <v>621</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B12" t="s">
-        <v>636</v>
+        <v>622</v>
       </c>
       <c r="C12" t="s">
-        <v>637</v>
+        <v>623</v>
       </c>
       <c r="D12" t="s">
-        <v>638</v>
+        <v>624</v>
       </c>
       <c r="E12" t="s">
-        <v>638</v>
+        <v>624</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
+        <v>612</v>
+      </c>
+      <c r="B13" t="s">
+        <v>625</v>
+      </c>
+      <c r="C13" t="s">
         <v>626</v>
       </c>
-      <c r="B13" t="s">
-        <v>639</v>
-      </c>
-      <c r="C13" t="s">
-        <v>640</v>
-      </c>
       <c r="D13" t="s">
-        <v>641</v>
+        <v>627</v>
       </c>
       <c r="E13" t="s">
-        <v>641</v>
+        <v>627</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B14" t="s">
-        <v>642</v>
+        <v>628</v>
       </c>
       <c r="C14" t="s">
-        <v>643</v>
+        <v>629</v>
       </c>
       <c r="D14" t="s">
-        <v>644</v>
+        <v>630</v>
       </c>
       <c r="E14" t="s">
-        <v>644</v>
+        <v>630</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B15" t="s">
-        <v>645</v>
+        <v>631</v>
       </c>
       <c r="C15" t="s">
-        <v>646</v>
+        <v>632</v>
       </c>
       <c r="D15" t="s">
-        <v>647</v>
+        <v>633</v>
       </c>
       <c r="E15" t="s">
-        <v>647</v>
+        <v>633</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B16" t="s">
-        <v>648</v>
+        <v>634</v>
       </c>
       <c r="C16" t="s">
-        <v>649</v>
+        <v>635</v>
       </c>
       <c r="D16" t="s">
-        <v>650</v>
+        <v>636</v>
       </c>
       <c r="E16" t="s">
-        <v>650</v>
+        <v>636</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B17" t="s">
-        <v>651</v>
+        <v>637</v>
       </c>
       <c r="C17" t="s">
-        <v>652</v>
+        <v>638</v>
       </c>
       <c r="D17" t="s">
-        <v>653</v>
+        <v>639</v>
       </c>
       <c r="E17" t="s">
-        <v>653</v>
+        <v>639</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B18" t="s">
-        <v>654</v>
+        <v>640</v>
       </c>
       <c r="C18" t="s">
-        <v>655</v>
+        <v>641</v>
       </c>
       <c r="D18" t="s">
-        <v>656</v>
+        <v>642</v>
       </c>
       <c r="E18" t="s">
-        <v>656</v>
+        <v>642</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B19" t="s">
-        <v>657</v>
+        <v>643</v>
       </c>
       <c r="C19" t="s">
-        <v>658</v>
+        <v>644</v>
       </c>
       <c r="D19" t="s">
-        <v>659</v>
+        <v>645</v>
       </c>
       <c r="E19" t="s">
-        <v>659</v>
+        <v>645</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B20" t="s">
-        <v>660</v>
+        <v>646</v>
       </c>
       <c r="C20" t="s">
-        <v>661</v>
+        <v>647</v>
       </c>
       <c r="D20" t="s">
-        <v>662</v>
+        <v>648</v>
       </c>
       <c r="E20" t="s">
-        <v>662</v>
+        <v>648</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B21" t="s">
-        <v>663</v>
+        <v>649</v>
       </c>
       <c r="C21" t="s">
-        <v>664</v>
+        <v>650</v>
       </c>
       <c r="D21" t="s">
-        <v>665</v>
+        <v>651</v>
       </c>
       <c r="E21" t="s">
-        <v>665</v>
+        <v>651</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B22" t="s">
-        <v>666</v>
+        <v>652</v>
       </c>
       <c r="C22" t="s">
-        <v>667</v>
+        <v>653</v>
       </c>
       <c r="D22" t="s">
-        <v>668</v>
+        <v>654</v>
       </c>
       <c r="E22" t="s">
-        <v>668</v>
+        <v>654</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B23" t="s">
-        <v>669</v>
+        <v>655</v>
       </c>
       <c r="C23" t="s">
-        <v>670</v>
+        <v>656</v>
       </c>
       <c r="D23" t="s">
-        <v>671</v>
+        <v>657</v>
       </c>
       <c r="E23" t="s">
-        <v>671</v>
+        <v>657</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B24" t="s">
-        <v>672</v>
+        <v>658</v>
       </c>
       <c r="C24" t="s">
-        <v>673</v>
+        <v>659</v>
       </c>
       <c r="D24" t="s">
-        <v>674</v>
+        <v>660</v>
       </c>
       <c r="E24" t="s">
-        <v>674</v>
+        <v>660</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B25" t="s">
-        <v>675</v>
+        <v>661</v>
       </c>
       <c r="C25" t="s">
-        <v>676</v>
+        <v>662</v>
       </c>
       <c r="D25" t="s">
-        <v>677</v>
+        <v>663</v>
       </c>
       <c r="E25" t="s">
-        <v>677</v>
+        <v>663</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B26" t="s">
-        <v>678</v>
+        <v>664</v>
       </c>
       <c r="C26" t="s">
-        <v>679</v>
+        <v>665</v>
       </c>
       <c r="D26" t="s">
-        <v>680</v>
+        <v>666</v>
       </c>
       <c r="E26" t="s">
-        <v>680</v>
+        <v>666</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B27" t="s">
-        <v>681</v>
+        <v>667</v>
       </c>
       <c r="C27" t="s">
-        <v>682</v>
+        <v>668</v>
       </c>
       <c r="D27" t="s">
-        <v>683</v>
+        <v>669</v>
       </c>
       <c r="E27" t="s">
-        <v>683</v>
+        <v>669</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B28" t="s">
-        <v>684</v>
+        <v>670</v>
       </c>
       <c r="C28" t="s">
-        <v>685</v>
+        <v>671</v>
       </c>
       <c r="D28" t="s">
-        <v>686</v>
+        <v>672</v>
       </c>
       <c r="E28" t="s">
-        <v>686</v>
+        <v>672</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B29" t="s">
-        <v>687</v>
+        <v>673</v>
       </c>
       <c r="C29" t="s">
-        <v>688</v>
+        <v>674</v>
       </c>
       <c r="D29" t="s">
-        <v>689</v>
+        <v>675</v>
       </c>
       <c r="E29" t="s">
-        <v>689</v>
+        <v>675</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B30" t="s">
-        <v>690</v>
+        <v>676</v>
       </c>
       <c r="C30" t="s">
-        <v>691</v>
+        <v>677</v>
       </c>
       <c r="D30" t="s">
-        <v>692</v>
+        <v>678</v>
       </c>
       <c r="E30" t="s">
-        <v>692</v>
+        <v>678</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B31" t="s">
-        <v>693</v>
+        <v>679</v>
       </c>
       <c r="C31" t="s">
-        <v>694</v>
+        <v>680</v>
       </c>
       <c r="D31" t="s">
-        <v>695</v>
+        <v>681</v>
       </c>
       <c r="E31" t="s">
-        <v>695</v>
+        <v>681</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B32" t="s">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="C32" t="s">
-        <v>697</v>
+        <v>683</v>
       </c>
       <c r="D32" t="s">
-        <v>698</v>
+        <v>684</v>
       </c>
       <c r="E32" t="s">
-        <v>698</v>
+        <v>684</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B33" t="s">
-        <v>699</v>
+        <v>685</v>
       </c>
       <c r="C33" t="s">
-        <v>700</v>
+        <v>686</v>
       </c>
       <c r="D33" t="s">
-        <v>701</v>
+        <v>687</v>
       </c>
       <c r="E33" t="s">
-        <v>701</v>
+        <v>687</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B34" t="s">
-        <v>702</v>
+        <v>688</v>
       </c>
       <c r="C34" t="s">
-        <v>703</v>
+        <v>689</v>
       </c>
       <c r="D34" t="s">
-        <v>704</v>
+        <v>690</v>
       </c>
       <c r="E34" t="s">
-        <v>704</v>
+        <v>690</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B35" t="s">
-        <v>705</v>
+        <v>691</v>
       </c>
       <c r="C35" t="s">
-        <v>706</v>
+        <v>692</v>
       </c>
       <c r="D35" t="s">
-        <v>707</v>
+        <v>693</v>
       </c>
       <c r="E35" t="s">
-        <v>707</v>
+        <v>693</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B36" t="s">
-        <v>708</v>
+        <v>694</v>
       </c>
       <c r="C36" t="s">
-        <v>709</v>
+        <v>695</v>
       </c>
       <c r="D36" t="s">
-        <v>710</v>
+        <v>696</v>
       </c>
       <c r="E36" t="s">
-        <v>710</v>
+        <v>696</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B37" t="s">
-        <v>711</v>
+        <v>697</v>
       </c>
       <c r="C37" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="D37" t="s">
-        <v>713</v>
+        <v>699</v>
       </c>
       <c r="E37" t="s">
-        <v>713</v>
+        <v>699</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B38" t="s">
-        <v>714</v>
+        <v>700</v>
       </c>
       <c r="C38" t="s">
-        <v>715</v>
+        <v>701</v>
       </c>
       <c r="D38" t="s">
-        <v>716</v>
+        <v>702</v>
       </c>
       <c r="E38" t="s">
-        <v>716</v>
+        <v>702</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B39" t="s">
-        <v>717</v>
+        <v>703</v>
       </c>
       <c r="C39" t="s">
-        <v>718</v>
+        <v>704</v>
       </c>
       <c r="D39" t="s">
-        <v>719</v>
+        <v>705</v>
       </c>
       <c r="E39" t="s">
-        <v>719</v>
+        <v>705</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B40" t="s">
-        <v>720</v>
+        <v>706</v>
       </c>
       <c r="C40" t="s">
-        <v>721</v>
+        <v>707</v>
       </c>
       <c r="D40" t="s">
-        <v>722</v>
+        <v>708</v>
       </c>
       <c r="E40" t="s">
-        <v>722</v>
+        <v>708</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="B41" t="s">
-        <v>723</v>
+        <v>709</v>
       </c>
       <c r="C41" t="s">
-        <v>724</v>
+        <v>710</v>
       </c>
       <c r="D41" t="s">
-        <v>725</v>
+        <v>711</v>
       </c>
       <c r="E41" t="s">
-        <v>725</v>
+        <v>711</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>726</v>
+        <v>712</v>
       </c>
       <c r="B42" t="s">
-        <v>727</v>
+        <v>713</v>
       </c>
       <c r="C42" t="s">
-        <v>616</v>
+        <v>602</v>
       </c>
       <c r="D42" t="s">
-        <v>617</v>
+        <v>603</v>
       </c>
       <c r="E42" t="s">
-        <v>618</v>
+        <v>604</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>726</v>
+        <v>712</v>
       </c>
       <c r="B43" t="s">
-        <v>728</v>
+        <v>714</v>
       </c>
       <c r="C43" t="s">
-        <v>619</v>
+        <v>605</v>
       </c>
       <c r="D43" t="s">
-        <v>620</v>
+        <v>606</v>
       </c>
       <c r="E43" t="s">
-        <v>621</v>
+        <v>607</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>729</v>
+        <v>715</v>
       </c>
       <c r="B44" t="s">
-        <v>730</v>
+        <v>716</v>
       </c>
       <c r="C44" t="s">
-        <v>731</v>
+        <v>717</v>
       </c>
       <c r="D44" t="s">
-        <v>732</v>
+        <v>718</v>
       </c>
       <c r="E44" t="s">
-        <v>733</v>
+        <v>719</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>729</v>
+        <v>715</v>
       </c>
       <c r="B45" t="s">
-        <v>734</v>
+        <v>720</v>
       </c>
       <c r="C45" t="s">
-        <v>735</v>
+        <v>721</v>
       </c>
       <c r="D45" t="s">
-        <v>736</v>
+        <v>722</v>
       </c>
       <c r="E45" t="s">
-        <v>737</v>
+        <v>723</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>738</v>
+        <v>724</v>
       </c>
       <c r="B46" t="s">
-        <v>739</v>
+        <v>725</v>
       </c>
       <c r="C46" t="s">
-        <v>740</v>
+        <v>726</v>
       </c>
       <c r="D46" t="s">
-        <v>741</v>
+        <v>727</v>
       </c>
       <c r="E46" t="s">
-        <v>742</v>
+        <v>728</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>738</v>
+        <v>724</v>
       </c>
       <c r="B47" t="s">
-        <v>743</v>
+        <v>729</v>
       </c>
       <c r="C47" t="s">
-        <v>744</v>
+        <v>730</v>
       </c>
       <c r="D47" t="s">
-        <v>745</v>
+        <v>731</v>
       </c>
       <c r="E47" t="s">
-        <v>746</v>
+        <v>732</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>557</v>
+        <v>544</v>
       </c>
       <c r="B48" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C48" t="s">
-        <v>747</v>
+        <v>733</v>
       </c>
       <c r="D48" t="s">
-        <v>748</v>
+        <v>734</v>
       </c>
       <c r="E48" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>557</v>
+        <v>544</v>
       </c>
       <c r="B49" t="s">
-        <v>610</v>
+        <v>596</v>
       </c>
       <c r="C49" t="s">
-        <v>750</v>
+        <v>736</v>
       </c>
       <c r="D49" t="s">
-        <v>751</v>
+        <v>737</v>
       </c>
       <c r="E49" t="s">
-        <v>752</v>
+        <v>738</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>557</v>
+        <v>544</v>
       </c>
       <c r="B50" t="s">
-        <v>622</v>
+        <v>608</v>
       </c>
       <c r="C50" t="s">
-        <v>753</v>
+        <v>739</v>
       </c>
       <c r="D50" t="s">
-        <v>754</v>
+        <v>740</v>
       </c>
       <c r="E50" t="s">
-        <v>755</v>
+        <v>741</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>557</v>
+        <v>544</v>
       </c>
       <c r="B51" t="s">
-        <v>633</v>
+        <v>619</v>
       </c>
       <c r="C51" t="s">
-        <v>756</v>
+        <v>742</v>
       </c>
       <c r="D51" t="s">
-        <v>757</v>
+        <v>743</v>
       </c>
       <c r="E51" t="s">
-        <v>758</v>
+        <v>744</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>759</v>
+        <v>745</v>
       </c>
       <c r="B52" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C52" t="s">
-        <v>616</v>
+        <v>602</v>
       </c>
       <c r="D52" t="s">
-        <v>617</v>
+        <v>603</v>
       </c>
       <c r="E52" t="s">
-        <v>618</v>
+        <v>604</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>759</v>
+        <v>745</v>
       </c>
       <c r="B53" t="s">
-        <v>610</v>
+        <v>596</v>
       </c>
       <c r="C53" t="s">
-        <v>760</v>
+        <v>746</v>
       </c>
       <c r="D53" t="s">
-        <v>761</v>
+        <v>747</v>
       </c>
       <c r="E53" t="s">
-        <v>762</v>
+        <v>748</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>759</v>
+        <v>745</v>
       </c>
       <c r="B54" t="s">
-        <v>622</v>
+        <v>608</v>
       </c>
       <c r="C54" t="s">
-        <v>763</v>
+        <v>749</v>
       </c>
       <c r="D54" t="s">
-        <v>764</v>
+        <v>750</v>
       </c>
       <c r="E54" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>766</v>
+        <v>752</v>
       </c>
       <c r="B55" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C55" t="s">
-        <v>616</v>
+        <v>602</v>
       </c>
       <c r="D55" t="s">
-        <v>617</v>
+        <v>603</v>
       </c>
       <c r="E55" t="s">
-        <v>618</v>
+        <v>604</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>766</v>
+        <v>752</v>
       </c>
       <c r="B56" t="s">
-        <v>610</v>
+        <v>596</v>
       </c>
       <c r="C56" t="s">
-        <v>767</v>
+        <v>753</v>
       </c>
       <c r="D56" t="s">
-        <v>768</v>
+        <v>754</v>
       </c>
       <c r="E56" t="s">
-        <v>769</v>
+        <v>755</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>766</v>
+        <v>752</v>
       </c>
       <c r="B57" t="s">
-        <v>622</v>
+        <v>608</v>
       </c>
       <c r="C57" t="s">
-        <v>770</v>
+        <v>756</v>
       </c>
       <c r="D57" t="s">
-        <v>771</v>
+        <v>757</v>
       </c>
       <c r="E57" t="s">
-        <v>772</v>
+        <v>758</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>773</v>
+        <v>759</v>
       </c>
       <c r="B58" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C58" t="s">
-        <v>774</v>
+        <v>760</v>
       </c>
       <c r="D58" t="s">
-        <v>775</v>
+        <v>761</v>
       </c>
       <c r="E58" t="s">
-        <v>776</v>
+        <v>762</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>773</v>
+        <v>759</v>
       </c>
       <c r="B59" t="s">
-        <v>610</v>
+        <v>596</v>
       </c>
       <c r="C59" t="s">
-        <v>777</v>
+        <v>763</v>
       </c>
       <c r="D59" t="s">
-        <v>778</v>
+        <v>764</v>
       </c>
       <c r="E59" t="s">
-        <v>779</v>
+        <v>765</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>780</v>
+        <v>766</v>
       </c>
       <c r="B60" t="s">
-        <v>633</v>
+        <v>619</v>
       </c>
       <c r="C60" t="s">
-        <v>781</v>
+        <v>767</v>
       </c>
       <c r="D60" t="s">
-        <v>782</v>
+        <v>768</v>
       </c>
       <c r="E60" t="s">
-        <v>783</v>
+        <v>769</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>780</v>
+        <v>766</v>
       </c>
       <c r="B61" t="s">
-        <v>636</v>
+        <v>622</v>
       </c>
       <c r="C61" t="s">
-        <v>784</v>
+        <v>770</v>
       </c>
       <c r="D61" t="s">
-        <v>785</v>
+        <v>771</v>
       </c>
       <c r="E61" t="s">
-        <v>786</v>
+        <v>772</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>787</v>
+        <v>773</v>
       </c>
       <c r="B62" t="s">
-        <v>622</v>
+        <v>608</v>
       </c>
       <c r="C62" t="s">
-        <v>788</v>
+        <v>774</v>
       </c>
       <c r="D62" t="s">
-        <v>789</v>
+        <v>775</v>
       </c>
       <c r="E62" t="s">
-        <v>790</v>
+        <v>776</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>791</v>
+        <v>777</v>
       </c>
       <c r="B63" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C63" t="s">
-        <v>616</v>
+        <v>602</v>
       </c>
       <c r="D63" t="s">
-        <v>617</v>
+        <v>603</v>
       </c>
       <c r="E63" t="s">
-        <v>618</v>
+        <v>604</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>791</v>
+        <v>777</v>
       </c>
       <c r="B64" t="s">
-        <v>792</v>
+        <v>778</v>
       </c>
       <c r="C64" t="s">
-        <v>619</v>
+        <v>605</v>
       </c>
       <c r="D64" t="s">
-        <v>620</v>
+        <v>606</v>
       </c>
       <c r="E64" t="s">
-        <v>621</v>
+        <v>607</v>
       </c>
     </row>
   </sheetData>
@@ -7272,36 +7172,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>793</v>
+        <v>779</v>
       </c>
       <c r="B1" t="s">
-        <v>794</v>
+        <v>780</v>
       </c>
       <c r="C1" t="s">
-        <v>795</v>
+        <v>781</v>
       </c>
       <c r="D1" t="s">
-        <v>796</v>
+        <v>782</v>
       </c>
       <c r="E1" t="s">
-        <v>797</v>
+        <v>783</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>798</v>
+        <v>784</v>
       </c>
       <c r="B2" t="s">
-        <v>798</v>
+        <v>784</v>
       </c>
       <c r="C2" t="s">
-        <v>799</v>
+        <v>785</v>
       </c>
       <c r="D2" t="s">
-        <v>800</v>
+        <v>786</v>
       </c>
       <c r="E2" t="s">
-        <v>801</v>
+        <v>787</v>
       </c>
     </row>
   </sheetData>

</xml_diff>